<commit_message>
Added Average Compression/Decompression Speeds
</commit_message>
<xml_diff>
--- a/research/compiled_data/Livro1.xlsx
+++ b/research/compiled_data/Livro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Silva\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEE0782-5435-4656-B0A2-10E80623F78F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EA5FE8D-A71D-4902-87A9-5E66D52E1B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="233" xr2:uid="{A8E8026A-0827-4328-8DB2-6CB64CB9D15B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="44">
   <si>
     <t>jpeg</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Melhor Geração</t>
+  </si>
+  <si>
+    <t>cmp10</t>
   </si>
 </sst>
 </file>
@@ -3390,6 +3393,759 @@
   <c:spPr>
     <a:solidFill>
       <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Velocidade</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> Média de compressão</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t>(MB/S)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:pattFill prst="narVert">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>Jpeg2000 Parte 1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Jpeg</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Bzip2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Png</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Cmp ger. 10</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$P$127:$T$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9578-4DF0-B828-E59C1552460F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="227"/>
+        <c:overlap val="-48"/>
+        <c:axId val="554323208"/>
+        <c:axId val="554320256"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="554323208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554320256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="554320256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554323208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT" sz="1800" b="1" i="0" cap="all" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Velocidade Média de descompressão</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT" sz="1800" b="1" i="0" cap="all" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(MB/S)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:pattFill prst="narVert">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>Jpeg2000 Parte 1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Jpeg</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Bzip2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Png</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Cmp ger. 10</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$P$135:$T$135</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E0C0-4766-B440-497601A2F02E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="227"/>
+        <c:overlap val="-48"/>
+        <c:axId val="554326816"/>
+        <c:axId val="554321240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="554326816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554321240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="554321240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554326816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -10156,6 +10912,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -12535,6 +13371,1044 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="217">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="217">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -17928,6 +19802,78 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1769B30-170E-4C01-97F9-B5AB4D72996F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>424542</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>119742</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>119742</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>87085</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF54970B-912B-446C-B64A-D4BF8257992B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -18620,10 +20566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8244EF-F26E-4B6C-9356-A1D409A957BC}">
-  <dimension ref="A1:AS113"/>
+  <dimension ref="A1:AS138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z70" sqref="Z70"/>
+    <sheetView tabSelected="1" topLeftCell="O103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH143" sqref="AH143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19517,7 +21463,7 @@
         <v>11.18</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="6"/>
+        <f>ROUND(J23,2)</f>
         <v>19.649999999999999</v>
       </c>
       <c r="AB23">
@@ -20134,7 +22080,7 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="AA34">
-        <f t="shared" si="7"/>
+        <f>ROUND(K34/1024/1024,2)</f>
         <v>4.59</v>
       </c>
       <c r="AB34">
@@ -22499,8 +24445,288 @@
     <row r="112" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F113" s="1"/>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" t="s">
+        <v>2</v>
+      </c>
+      <c r="E126" t="s">
+        <v>8</v>
+      </c>
+      <c r="F126" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="B127">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="C127">
+        <v>0.25</v>
+      </c>
+      <c r="D127">
+        <v>1.38</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127" s="1">
+        <v>19.649999999999999</v>
+      </c>
+      <c r="H127">
+        <f>ROUND((A127+A128+A129+A130)/4,1)</f>
+        <v>22.2</v>
+      </c>
+      <c r="I127">
+        <f>ROUND((B127+B128+B129+B130)/4,1)</f>
+        <v>6</v>
+      </c>
+      <c r="J127">
+        <f t="shared" ref="I127:M127" si="18">ROUND((C127+C128+C129+C130)/4,1)</f>
+        <v>0.3</v>
+      </c>
+      <c r="K127">
+        <f t="shared" si="18"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L127">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="M127">
+        <f t="shared" si="18"/>
+        <v>17.8</v>
+      </c>
+      <c r="P127">
+        <f>ROUND((22.2/I127),1)</f>
+        <v>3.7</v>
+      </c>
+      <c r="Q127">
+        <f t="shared" ref="Q127:V127" si="19">ROUND((22.2/J127),1)</f>
+        <v>74</v>
+      </c>
+      <c r="R127">
+        <f t="shared" si="19"/>
+        <v>20.2</v>
+      </c>
+      <c r="S127">
+        <v>0</v>
+      </c>
+      <c r="T127">
+        <f t="shared" si="19"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>10.4</v>
+      </c>
+      <c r="B128">
+        <v>3.54</v>
+      </c>
+      <c r="C128">
+        <v>0.15</v>
+      </c>
+      <c r="D128">
+        <v>0.97</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128" s="1">
+        <v>14.86</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>45.7</v>
+      </c>
+      <c r="B129">
+        <v>9.92</v>
+      </c>
+      <c r="C129">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D129">
+        <v>0.89</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129" s="1">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>15.9</v>
+      </c>
+      <c r="B130">
+        <v>5.42</v>
+      </c>
+      <c r="C130">
+        <v>0.25</v>
+      </c>
+      <c r="D130">
+        <v>1.21</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130" s="1">
+        <v>21.22</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" t="s">
+        <v>0</v>
+      </c>
+      <c r="D134" t="s">
+        <v>2</v>
+      </c>
+      <c r="E134" t="s">
+        <v>8</v>
+      </c>
+      <c r="F134" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="B135">
+        <v>4.03</v>
+      </c>
+      <c r="C135">
+        <v>0.19</v>
+      </c>
+      <c r="D135">
+        <v>0.89</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135">
+        <v>0.79</v>
+      </c>
+      <c r="H135">
+        <f>ROUND((A135+A136+A137+A138)/4,1)</f>
+        <v>22.2</v>
+      </c>
+      <c r="I135">
+        <f t="shared" ref="I135:M135" si="20">ROUND((B135+B136+B137+B138)/4,1)</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J135">
+        <f t="shared" si="20"/>
+        <v>0.2</v>
+      </c>
+      <c r="K135">
+        <f t="shared" si="20"/>
+        <v>0.8</v>
+      </c>
+      <c r="L135">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="M135">
+        <f t="shared" si="20"/>
+        <v>0.8</v>
+      </c>
+      <c r="P135">
+        <f>ROUND(22.2/I135,1)</f>
+        <v>4.5</v>
+      </c>
+      <c r="Q135">
+        <f t="shared" ref="Q135:T135" si="21">ROUND(22.2/J135,1)</f>
+        <v>111</v>
+      </c>
+      <c r="R135">
+        <f t="shared" si="21"/>
+        <v>27.8</v>
+      </c>
+      <c r="S135">
+        <v>0</v>
+      </c>
+      <c r="T135">
+        <f t="shared" si="21"/>
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>10.4</v>
+      </c>
+      <c r="B136">
+        <v>2.83</v>
+      </c>
+      <c r="C136">
+        <v>0.12</v>
+      </c>
+      <c r="D136">
+        <v>0.61</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="F136">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>45.7</v>
+      </c>
+      <c r="B137">
+        <v>8.59</v>
+      </c>
+      <c r="C137">
+        <v>0.42</v>
+      </c>
+      <c r="D137">
+        <v>0.68</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>15.9</v>
+      </c>
+      <c r="B138">
+        <v>4.33</v>
+      </c>
+      <c r="C138">
+        <v>0.19</v>
+      </c>
+      <c r="D138">
+        <v>0.86</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <v>0.95</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code Documentation corrections and Code Revision.
</commit_message>
<xml_diff>
--- a/research/compiled_data/Livro1.xlsx
+++ b/research/compiled_data/Livro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Silva\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEE0782-5435-4656-B0A2-10E80623F78F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EA5FE8D-A71D-4902-87A9-5E66D52E1B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="233" xr2:uid="{A8E8026A-0827-4328-8DB2-6CB64CB9D15B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="44">
   <si>
     <t>jpeg</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Melhor Geração</t>
+  </si>
+  <si>
+    <t>cmp10</t>
   </si>
 </sst>
 </file>
@@ -3390,6 +3393,759 @@
   <c:spPr>
     <a:solidFill>
       <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Velocidade</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> Média de compressão</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t>(MB/S)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:pattFill prst="narVert">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>Jpeg2000 Parte 1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Jpeg</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Bzip2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Png</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Cmp ger. 10</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$P$127:$T$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9578-4DF0-B828-E59C1552460F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="227"/>
+        <c:overlap val="-48"/>
+        <c:axId val="554323208"/>
+        <c:axId val="554320256"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="554323208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554320256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="554320256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554323208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT" sz="1800" b="1" i="0" cap="all" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Velocidade Média de descompressão</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT" sz="1800" b="1" i="0" cap="all" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(MB/S)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:pattFill prst="narVert">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>Jpeg2000 Parte 1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Jpeg</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Bzip2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Png</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Cmp ger. 10</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$P$135:$T$135</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E0C0-4766-B440-497601A2F02E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="227"/>
+        <c:overlap val="-48"/>
+        <c:axId val="554326816"/>
+        <c:axId val="554321240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="554326816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554321240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="554321240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554326816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -10156,6 +10912,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -12535,6 +13371,1044 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="217">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="217">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -17928,6 +19802,78 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1769B30-170E-4C01-97F9-B5AB4D72996F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>424542</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>119742</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>119742</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>87085</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF54970B-912B-446C-B64A-D4BF8257992B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -18620,10 +20566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8244EF-F26E-4B6C-9356-A1D409A957BC}">
-  <dimension ref="A1:AS113"/>
+  <dimension ref="A1:AS138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z70" sqref="Z70"/>
+    <sheetView tabSelected="1" topLeftCell="O103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH143" sqref="AH143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19517,7 +21463,7 @@
         <v>11.18</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="6"/>
+        <f>ROUND(J23,2)</f>
         <v>19.649999999999999</v>
       </c>
       <c r="AB23">
@@ -20134,7 +22080,7 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="AA34">
-        <f t="shared" si="7"/>
+        <f>ROUND(K34/1024/1024,2)</f>
         <v>4.59</v>
       </c>
       <c r="AB34">
@@ -22499,8 +24445,288 @@
     <row r="112" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F113" s="1"/>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" t="s">
+        <v>2</v>
+      </c>
+      <c r="E126" t="s">
+        <v>8</v>
+      </c>
+      <c r="F126" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="B127">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="C127">
+        <v>0.25</v>
+      </c>
+      <c r="D127">
+        <v>1.38</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127" s="1">
+        <v>19.649999999999999</v>
+      </c>
+      <c r="H127">
+        <f>ROUND((A127+A128+A129+A130)/4,1)</f>
+        <v>22.2</v>
+      </c>
+      <c r="I127">
+        <f>ROUND((B127+B128+B129+B130)/4,1)</f>
+        <v>6</v>
+      </c>
+      <c r="J127">
+        <f t="shared" ref="I127:M127" si="18">ROUND((C127+C128+C129+C130)/4,1)</f>
+        <v>0.3</v>
+      </c>
+      <c r="K127">
+        <f t="shared" si="18"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L127">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="M127">
+        <f t="shared" si="18"/>
+        <v>17.8</v>
+      </c>
+      <c r="P127">
+        <f>ROUND((22.2/I127),1)</f>
+        <v>3.7</v>
+      </c>
+      <c r="Q127">
+        <f t="shared" ref="Q127:V127" si="19">ROUND((22.2/J127),1)</f>
+        <v>74</v>
+      </c>
+      <c r="R127">
+        <f t="shared" si="19"/>
+        <v>20.2</v>
+      </c>
+      <c r="S127">
+        <v>0</v>
+      </c>
+      <c r="T127">
+        <f t="shared" si="19"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>10.4</v>
+      </c>
+      <c r="B128">
+        <v>3.54</v>
+      </c>
+      <c r="C128">
+        <v>0.15</v>
+      </c>
+      <c r="D128">
+        <v>0.97</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128" s="1">
+        <v>14.86</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>45.7</v>
+      </c>
+      <c r="B129">
+        <v>9.92</v>
+      </c>
+      <c r="C129">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D129">
+        <v>0.89</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129" s="1">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>15.9</v>
+      </c>
+      <c r="B130">
+        <v>5.42</v>
+      </c>
+      <c r="C130">
+        <v>0.25</v>
+      </c>
+      <c r="D130">
+        <v>1.21</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130" s="1">
+        <v>21.22</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" t="s">
+        <v>0</v>
+      </c>
+      <c r="D134" t="s">
+        <v>2</v>
+      </c>
+      <c r="E134" t="s">
+        <v>8</v>
+      </c>
+      <c r="F134" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="B135">
+        <v>4.03</v>
+      </c>
+      <c r="C135">
+        <v>0.19</v>
+      </c>
+      <c r="D135">
+        <v>0.89</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135">
+        <v>0.79</v>
+      </c>
+      <c r="H135">
+        <f>ROUND((A135+A136+A137+A138)/4,1)</f>
+        <v>22.2</v>
+      </c>
+      <c r="I135">
+        <f t="shared" ref="I135:M135" si="20">ROUND((B135+B136+B137+B138)/4,1)</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J135">
+        <f t="shared" si="20"/>
+        <v>0.2</v>
+      </c>
+      <c r="K135">
+        <f t="shared" si="20"/>
+        <v>0.8</v>
+      </c>
+      <c r="L135">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="M135">
+        <f t="shared" si="20"/>
+        <v>0.8</v>
+      </c>
+      <c r="P135">
+        <f>ROUND(22.2/I135,1)</f>
+        <v>4.5</v>
+      </c>
+      <c r="Q135">
+        <f t="shared" ref="Q135:T135" si="21">ROUND(22.2/J135,1)</f>
+        <v>111</v>
+      </c>
+      <c r="R135">
+        <f t="shared" si="21"/>
+        <v>27.8</v>
+      </c>
+      <c r="S135">
+        <v>0</v>
+      </c>
+      <c r="T135">
+        <f t="shared" si="21"/>
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>10.4</v>
+      </c>
+      <c r="B136">
+        <v>2.83</v>
+      </c>
+      <c r="C136">
+        <v>0.12</v>
+      </c>
+      <c r="D136">
+        <v>0.61</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="F136">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>45.7</v>
+      </c>
+      <c r="B137">
+        <v>8.59</v>
+      </c>
+      <c r="C137">
+        <v>0.42</v>
+      </c>
+      <c r="D137">
+        <v>0.68</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>15.9</v>
+      </c>
+      <c r="B138">
+        <v>4.33</v>
+      </c>
+      <c r="C138">
+        <v>0.19</v>
+      </c>
+      <c r="D138">
+        <v>0.86</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <v>0.95</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added some fixes to the compiled data Excel
</commit_message>
<xml_diff>
--- a/research/compiled_data/Livro1.xlsx
+++ b/research/compiled_data/Livro1.xlsx
@@ -5,29 +5,20 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Silva\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sancho\Desktop\TI-TP2\research\compiled_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EA5FE8D-A71D-4902-87A9-5E66D52E1B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E9EE12-1D42-4989-BF2E-3DBDA99E7A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="233" xr2:uid="{A8E8026A-0827-4328-8DB2-6CB64CB9D15B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="233" xr2:uid="{A8E8026A-0827-4328-8DB2-6CB64CB9D15B}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -281,7 +272,7 @@
               <a:rPr lang="pt-PT" sz="1800" b="1" i="0" cap="all" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>(segundos)</a:t>
+              <a:t>(s)</a:t>
             </a:r>
             <a:endParaRPr lang="pt-PT">
               <a:effectLst/>
@@ -1082,7 +1073,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-PT" sz="1800"/>
-              <a:t>(segundos)</a:t>
+              <a:t>(s)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1880,7 +1871,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-PT" sz="1800"/>
-              <a:t>(Segundos)</a:t>
+              <a:t>(S)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2669,7 +2660,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-PT" sz="2000"/>
-              <a:t>Taxa de Compressão</a:t>
+              <a:t>Taxa de Compressão (S)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5020,7 +5011,7 @@
               <a:rPr lang="pt-PT" sz="1800" b="1" i="0" cap="all" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>TAxa de compressão</a:t>
+              <a:t>TAxa de compressão (%)</a:t>
             </a:r>
             <a:endParaRPr lang="pt-PT">
               <a:effectLst/>
@@ -5784,7 +5775,7 @@
               <a:rPr lang="pt-PT" sz="1800" b="1" i="0" cap="all" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>(segundos)</a:t>
+              <a:t>(s)</a:t>
             </a:r>
             <a:endParaRPr lang="pt-PT">
               <a:effectLst/>
@@ -7676,7 +7667,7 @@
               <a:rPr lang="pt-PT" sz="1800" b="1" i="0" cap="all" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>(segundos)</a:t>
+              <a:t>(S)</a:t>
             </a:r>
             <a:endParaRPr lang="pt-PT">
               <a:effectLst/>
@@ -10041,7 +10032,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-PT" sz="1800" baseline="0"/>
-              <a:t>(Segundos)</a:t>
+              <a:t>(S)</a:t>
             </a:r>
             <a:endParaRPr lang="pt-PT" sz="1800"/>
           </a:p>
@@ -19336,8 +19327,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>76199</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>87085</xdr:rowOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>117231</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19371,9 +19362,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>58</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>117021</xdr:rowOff>
+      <xdr:colOff>293077</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>146538</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19407,9 +19398,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>163285</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
+      <xdr:colOff>175846</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>109904</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19436,16 +19427,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>130628</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>534866</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>119741</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>435428</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>87084</xdr:rowOff>
+      <xdr:colOff>435429</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>109904</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19473,15 +19464,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:colOff>168521</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>65314</xdr:rowOff>
+      <xdr:rowOff>123929</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>32657</xdr:rowOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>578828</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>168519</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19509,15 +19500,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>261852</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>172539</xdr:rowOff>
+      <xdr:colOff>217890</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>121250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>566652</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>150272</xdr:rowOff>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>36635</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>153865</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20568,18 +20559,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8244EF-F26E-4B6C-9356-A1D409A957BC}">
   <dimension ref="A1:AS138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH143" sqref="AH143"/>
+    <sheetView tabSelected="1" topLeftCell="AC74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O60" sqref="O60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="K1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -20611,7 +20602,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>16.899999999999999</v>
       </c>
@@ -20673,7 +20664,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10.4</v>
       </c>
@@ -20738,7 +20729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>45.7</v>
       </c>
@@ -20803,7 +20794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15.9</v>
       </c>
@@ -20880,7 +20871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="K7">
         <v>7.45</v>
       </c>
@@ -20924,7 +20915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="AO8" t="s">
         <v>37</v>
       </c>
@@ -20941,7 +20932,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
         <v>19</v>
       </c>
@@ -20949,7 +20940,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -21005,7 +20996,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -21052,7 +21043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -21121,7 +21112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -21190,7 +21181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -21259,7 +21250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -21286,7 +21277,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -21336,7 +21327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -21380,7 +21371,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22.09</v>
       </c>
@@ -21482,7 +21473,7 @@
         <v>41.81</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16.010000000000002</v>
       </c>
@@ -21584,7 +21575,7 @@
         <v>34.17</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20.29</v>
       </c>
@@ -21686,7 +21677,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>21.77</v>
       </c>
@@ -21788,7 +21779,7 @@
         <v>43.27</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.46</v>
       </c>
@@ -21890,7 +21881,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -21940,7 +21931,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0</v>
       </c>
@@ -21990,7 +21981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7189899</v>
       </c>
@@ -22100,7 +22091,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4853897</v>
       </c>
@@ -22210,7 +22201,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2775240</v>
       </c>
@@ -22320,7 +22311,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8876074</v>
       </c>
@@ -22430,7 +22421,7 @@
         <v>4.57</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>225908</v>
       </c>
@@ -22540,7 +22531,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -22590,7 +22581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -22634,7 +22625,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>67.55</v>
       </c>
@@ -22736,7 +22727,7 @@
         <v>76.510000000000005</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>63.4</v>
       </c>
@@ -22838,7 +22829,7 @@
         <v>73.540000000000006</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>94.26</v>
       </c>
@@ -22940,7 +22931,7 @@
         <v>95.62</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>61.26</v>
       </c>
@@ -23042,7 +23033,7 @@
         <v>71.39</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>40.32</v>
       </c>
@@ -23144,7 +23135,7 @@
         <v>36.25</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="Q48">
         <v>0</v>
       </c>
@@ -23191,12 +23182,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="49" spans="15:31" x14ac:dyDescent="0.25">
       <c r="Q49" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="50" spans="15:31" x14ac:dyDescent="0.25">
       <c r="P50" t="s">
         <v>3</v>
       </c>
@@ -23246,7 +23237,7 @@
         <v>75.069999999999993</v>
       </c>
     </row>
-    <row r="51" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="51" spans="15:31" x14ac:dyDescent="0.25">
       <c r="P51" t="s">
         <v>4</v>
       </c>
@@ -23296,7 +23287,7 @@
         <v>57.29</v>
       </c>
     </row>
-    <row r="52" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="52" spans="15:31" x14ac:dyDescent="0.25">
       <c r="P52" t="s">
         <v>5</v>
       </c>
@@ -23346,7 +23337,7 @@
         <v>153.85</v>
       </c>
     </row>
-    <row r="53" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="53" spans="15:31" x14ac:dyDescent="0.25">
       <c r="P53" t="s">
         <v>6</v>
       </c>
@@ -23396,7 +23387,7 @@
         <v>79.23</v>
       </c>
     </row>
-    <row r="54" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="54" spans="15:31" x14ac:dyDescent="0.25">
       <c r="P54" t="s">
         <v>13</v>
       </c>
@@ -23446,7 +23437,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="57" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="57" spans="15:31" x14ac:dyDescent="0.25">
       <c r="Q57">
         <v>0</v>
       </c>
@@ -23493,7 +23484,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="58" spans="15:31" x14ac:dyDescent="0.25">
       <c r="O58" t="s">
         <v>22</v>
       </c>
@@ -23558,7 +23549,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="59" spans="15:31" x14ac:dyDescent="0.25">
       <c r="O59" t="s">
         <v>23</v>
       </c>
@@ -23623,7 +23614,7 @@
         <v>91.4</v>
       </c>
     </row>
-    <row r="60" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="60" spans="15:31" x14ac:dyDescent="0.25">
       <c r="O60" t="s">
         <v>27</v>
       </c>
@@ -23688,7 +23679,7 @@
         <v>127.4</v>
       </c>
     </row>
-    <row r="62" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="62" spans="15:31" x14ac:dyDescent="0.25">
       <c r="O62" t="s">
         <v>24</v>
       </c>
@@ -23753,7 +23744,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="64" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="64" spans="15:31" x14ac:dyDescent="0.25">
       <c r="O64" t="s">
         <v>25</v>
       </c>
@@ -23818,7 +23809,7 @@
         <v>70.7</v>
       </c>
     </row>
-    <row r="68" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="68" spans="15:31" x14ac:dyDescent="0.25">
       <c r="Q68">
         <v>0</v>
       </c>
@@ -23865,12 +23856,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="69" spans="15:31" x14ac:dyDescent="0.25">
       <c r="Q69" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="70" spans="15:31" x14ac:dyDescent="0.25">
       <c r="P70" t="s">
         <v>3</v>
       </c>
@@ -23935,7 +23926,7 @@
         <v>116.9</v>
       </c>
     </row>
-    <row r="71" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="71" spans="15:31" x14ac:dyDescent="0.25">
       <c r="P71" t="s">
         <v>4</v>
       </c>
@@ -24000,7 +23991,7 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="72" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="72" spans="15:31" x14ac:dyDescent="0.25">
       <c r="P72" t="s">
         <v>5</v>
       </c>
@@ -24065,7 +24056,7 @@
         <v>178.6</v>
       </c>
     </row>
-    <row r="73" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="73" spans="15:31" x14ac:dyDescent="0.25">
       <c r="P73" t="s">
         <v>6</v>
       </c>
@@ -24130,7 +24121,7 @@
         <v>122.5</v>
       </c>
     </row>
-    <row r="74" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="74" spans="15:31" x14ac:dyDescent="0.25">
       <c r="P74" t="s">
         <v>13</v>
       </c>
@@ -24195,7 +24186,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="76" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="76" spans="15:31" x14ac:dyDescent="0.25">
       <c r="Q76">
         <v>0</v>
       </c>
@@ -24242,7 +24233,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="15:31" x14ac:dyDescent="0.3">
+    <row r="77" spans="15:31" x14ac:dyDescent="0.25">
       <c r="O77" t="s">
         <v>42</v>
       </c>
@@ -24307,12 +24298,12 @@
         <v>42.1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>1</v>
       </c>
@@ -24332,7 +24323,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -24355,7 +24346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>4</v>
       </c>
@@ -24378,7 +24369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -24401,7 +24392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -24424,31 +24415,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F107" s="1"/>
     </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F113" s="1"/>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>1</v>
       </c>
@@ -24465,7 +24456,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>16.899999999999999</v>
       </c>
@@ -24493,7 +24484,7 @@
         <v>6</v>
       </c>
       <c r="J127">
-        <f t="shared" ref="I127:M127" si="18">ROUND((C127+C128+C129+C130)/4,1)</f>
+        <f t="shared" ref="J127:M127" si="18">ROUND((C127+C128+C129+C130)/4,1)</f>
         <v>0.3</v>
       </c>
       <c r="K127">
@@ -24513,7 +24504,7 @@
         <v>3.7</v>
       </c>
       <c r="Q127">
-        <f t="shared" ref="Q127:V127" si="19">ROUND((22.2/J127),1)</f>
+        <f t="shared" ref="Q127:T127" si="19">ROUND((22.2/J127),1)</f>
         <v>74</v>
       </c>
       <c r="R127">
@@ -24528,7 +24519,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>10.4</v>
       </c>
@@ -24548,7 +24539,7 @@
         <v>14.86</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>45.7</v>
       </c>
@@ -24568,7 +24559,7 @@
         <v>15.62</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>15.9</v>
       </c>
@@ -24588,7 +24579,7 @@
         <v>21.22</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>1</v>
       </c>
@@ -24605,7 +24596,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>16.899999999999999</v>
       </c>
@@ -24668,7 +24659,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>10.4</v>
       </c>
@@ -24688,7 +24679,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>45.7</v>
       </c>
@@ -24708,7 +24699,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>15.9</v>
       </c>

</xml_diff>

<commit_message>
Added comparison graph between CMP10 and other algorithms
</commit_message>
<xml_diff>
--- a/research/compiled_data/Livro1.xlsx
+++ b/research/compiled_data/Livro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Silva\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96212BDB-2DAA-43F8-83FE-97C5AFB833E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EED70F5-BE41-44F1-907B-D11B74097E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="233" xr2:uid="{A8E8026A-0827-4328-8DB2-6CB64CB9D15B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="48">
   <si>
     <t>jpeg</t>
   </si>
@@ -176,6 +176,9 @@
   <si>
     <t>MEDIA</t>
   </si>
+  <si>
+    <t>cmp 10</t>
+  </si>
 </sst>
 </file>
 
@@ -217,10 +220,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5022,6 +5031,519 @@
   <c:spPr>
     <a:solidFill>
       <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Comparação do Cmp ger.10</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>com</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> outros algoritmos</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Média da Taxa de Compressão</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>Jpeg2000 Parte 1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Jpeg</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Bzip2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Png</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Cmp10</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$A$200:$E$200</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>78.260000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76.400000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-757D-44EF-9527-5F906AE74FD5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Média do Tempo Total</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>Jpeg2000 Parte 1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Jpeg</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Bzip2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Png</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Cmp10</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$A$201:$E$201</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10.91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.600000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-757D-44EF-9527-5F906AE74FD5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
+        <c:axId val="1260406696"/>
+        <c:axId val="1260407024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1260406696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1260407024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1260407024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1260406696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -12916,6 +13438,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -16852,6 +17414,530 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -23061,6 +24147,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>108856</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>21770</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE606943-5B6D-4125-966A-862378B307B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -23753,10 +24875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8244EF-F26E-4B6C-9356-A1D409A957BC}">
-  <dimension ref="A1:AS138"/>
+  <dimension ref="A1:AS201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X86" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF50" sqref="AF50"/>
+    <sheetView tabSelected="1" topLeftCell="A238" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F172" sqref="F172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24073,11 +25195,11 @@
         <v>5.2012999999999998</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:O7" si="2">ROUND((L3+L4+L5+L6)/4,4)</f>
+        <f>ROUND((L3+L4+L5+L6)/4,4)</f>
         <v>2.3289</v>
       </c>
       <c r="M7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="M7:O7" si="2">ROUND((M3+M4+M5+M6)/4,4)</f>
         <v>1.9454</v>
       </c>
       <c r="N7">
@@ -25927,7 +27049,7 @@
         <v>76.510000000000005</v>
       </c>
       <c r="AF42">
-        <f t="shared" si="12"/>
+        <f>ROUND((Q42+R42+S42+T42+U42+V42+W42+X42+Y42+Z42+AA42+AB42+AC42+AD42+AE42)/15,2)</f>
         <v>69.650000000000006</v>
       </c>
     </row>
@@ -26392,7 +27514,7 @@
         <v>75.069999999999993</v>
       </c>
       <c r="AF50">
-        <f t="shared" si="12"/>
+        <f>ROUND((Q50+R50+S50+T50+U50+V50+W50+X50+Y50+Z50+AA50+AB50+AC50+AD50+AE50)/15,2)</f>
         <v>44.34</v>
       </c>
     </row>
@@ -27856,7 +28978,647 @@
         <v>14.5</v>
       </c>
     </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B158" t="s">
+        <v>1</v>
+      </c>
+      <c r="C158" t="s">
+        <v>0</v>
+      </c>
+      <c r="D158" t="s">
+        <v>2</v>
+      </c>
+      <c r="E158" t="s">
+        <v>8</v>
+      </c>
+      <c r="F158" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="B159">
+        <v>3.98</v>
+      </c>
+      <c r="C159">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="D159">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="E159">
+        <v>4.41</v>
+      </c>
+      <c r="F159" s="1">
+        <v>4.59</v>
+      </c>
+      <c r="G159" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>10.4</v>
+      </c>
+      <c r="B160">
+        <v>3.06</v>
+      </c>
+      <c r="C160">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="D160">
+        <v>3.33</v>
+      </c>
+      <c r="E160">
+        <v>3.17</v>
+      </c>
+      <c r="F160" s="1">
+        <v>2.87</v>
+      </c>
+      <c r="G160" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>45.7</v>
+      </c>
+      <c r="B161">
+        <v>2.65</v>
+      </c>
+      <c r="C161">
+        <v>1.06</v>
+      </c>
+      <c r="D161">
+        <v>1.72</v>
+      </c>
+      <c r="E161">
+        <v>2.17</v>
+      </c>
+      <c r="F161" s="1">
+        <v>2.44</v>
+      </c>
+      <c r="G161" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>15.9</v>
+      </c>
+      <c r="B162">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="C162">
+        <v>0.98</v>
+      </c>
+      <c r="D162">
+        <v>5.36</v>
+      </c>
+      <c r="E162">
+        <v>5.21</v>
+      </c>
+      <c r="F162" s="1">
+        <v>5.55</v>
+      </c>
+      <c r="G162" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B167" t="s">
+        <v>1</v>
+      </c>
+      <c r="C167" t="s">
+        <v>0</v>
+      </c>
+      <c r="D167" t="s">
+        <v>2</v>
+      </c>
+      <c r="E167" t="s">
+        <v>8</v>
+      </c>
+      <c r="F167" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>3</v>
+      </c>
+      <c r="B169">
+        <v>76.45</v>
+      </c>
+      <c r="C169">
+        <v>94.43</v>
+      </c>
+      <c r="D169">
+        <v>73.25</v>
+      </c>
+      <c r="E169">
+        <v>73.91</v>
+      </c>
+      <c r="F169" s="1">
+        <v>72.87</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>4</v>
+      </c>
+      <c r="B170">
+        <v>70.58</v>
+      </c>
+      <c r="C170">
+        <v>96.9</v>
+      </c>
+      <c r="D170">
+        <v>67.98</v>
+      </c>
+      <c r="E170">
+        <v>69.52</v>
+      </c>
+      <c r="F170" s="1">
+        <v>72.650000000000006</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>5</v>
+      </c>
+      <c r="B171">
+        <v>94.2</v>
+      </c>
+      <c r="C171">
+        <v>97.68</v>
+      </c>
+      <c r="D171">
+        <v>96.24</v>
+      </c>
+      <c r="E171">
+        <v>95.25</v>
+      </c>
+      <c r="F171" s="1">
+        <v>94.67</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>6</v>
+      </c>
+      <c r="B172">
+        <v>71.819999999999993</v>
+      </c>
+      <c r="C172">
+        <v>93.84</v>
+      </c>
+      <c r="D172">
+        <v>66.290000000000006</v>
+      </c>
+      <c r="E172">
+        <v>67.23</v>
+      </c>
+      <c r="F172" s="1">
+        <v>65.209999999999994</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>44</v>
+      </c>
+      <c r="B173">
+        <f>ROUND((B169+B170+B171+B172)/4,2)</f>
+        <v>78.260000000000005</v>
+      </c>
+      <c r="C173">
+        <f t="shared" ref="C173:E173" si="30">ROUND((C169+C170+C171+C172)/4,2)</f>
+        <v>95.71</v>
+      </c>
+      <c r="D173">
+        <f t="shared" si="30"/>
+        <v>75.94</v>
+      </c>
+      <c r="E173">
+        <f t="shared" si="30"/>
+        <v>76.48</v>
+      </c>
+      <c r="F173" s="2">
+        <v>76.400000000000006</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B176" t="s">
+        <v>1</v>
+      </c>
+      <c r="C176" t="s">
+        <v>0</v>
+      </c>
+      <c r="D176" t="s">
+        <v>2</v>
+      </c>
+      <c r="E176" t="s">
+        <v>8</v>
+      </c>
+      <c r="F176" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>3</v>
+      </c>
+      <c r="B177">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="C177">
+        <v>0.25</v>
+      </c>
+      <c r="D177">
+        <v>1.38</v>
+      </c>
+      <c r="E177">
+        <v>0</v>
+      </c>
+      <c r="F177" s="1">
+        <v>19.649999999999999</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>4</v>
+      </c>
+      <c r="B178">
+        <v>3.54</v>
+      </c>
+      <c r="C178">
+        <v>0.15</v>
+      </c>
+      <c r="D178">
+        <v>0.97</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+      <c r="F178" s="1">
+        <v>14.86</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>5</v>
+      </c>
+      <c r="B179">
+        <v>9.92</v>
+      </c>
+      <c r="C179">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D179">
+        <v>0.89</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+      <c r="F179" s="1">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>6</v>
+      </c>
+      <c r="B180">
+        <v>5.42</v>
+      </c>
+      <c r="C180">
+        <v>0.25</v>
+      </c>
+      <c r="D180">
+        <v>1.21</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+      <c r="F180" s="1">
+        <v>21.22</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>44</v>
+      </c>
+      <c r="B181">
+        <v>5.97</v>
+      </c>
+      <c r="C181">
+        <v>0.31</v>
+      </c>
+      <c r="D181">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E181">
+        <v>0</v>
+      </c>
+      <c r="F181" s="2">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B184" t="s">
+        <v>1</v>
+      </c>
+      <c r="C184" t="s">
+        <v>0</v>
+      </c>
+      <c r="D184" t="s">
+        <v>2</v>
+      </c>
+      <c r="E184" t="s">
+        <v>8</v>
+      </c>
+      <c r="F184" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>3</v>
+      </c>
+      <c r="B185">
+        <v>4.03</v>
+      </c>
+      <c r="C185">
+        <v>0.19</v>
+      </c>
+      <c r="D185">
+        <v>0.89</v>
+      </c>
+      <c r="E185">
+        <v>0</v>
+      </c>
+      <c r="F185">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>4</v>
+      </c>
+      <c r="B186">
+        <v>2.83</v>
+      </c>
+      <c r="C186">
+        <v>0.12</v>
+      </c>
+      <c r="D186">
+        <v>0.61</v>
+      </c>
+      <c r="E186">
+        <v>0</v>
+      </c>
+      <c r="F186">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>5</v>
+      </c>
+      <c r="B187">
+        <v>8.59</v>
+      </c>
+      <c r="C187">
+        <v>0.42</v>
+      </c>
+      <c r="D187">
+        <v>0.68</v>
+      </c>
+      <c r="E187">
+        <v>0</v>
+      </c>
+      <c r="F187">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>6</v>
+      </c>
+      <c r="B188">
+        <v>4.33</v>
+      </c>
+      <c r="C188">
+        <v>0.19</v>
+      </c>
+      <c r="D188">
+        <v>0.86</v>
+      </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
+      <c r="F188">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>46</v>
+      </c>
+      <c r="B189">
+        <v>4.95</v>
+      </c>
+      <c r="C189">
+        <v>0.23</v>
+      </c>
+      <c r="D189">
+        <v>0.76</v>
+      </c>
+      <c r="E189">
+        <v>0</v>
+      </c>
+      <c r="F189" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A191" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B191" s="3"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B192" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F192" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A193" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B193" s="1">
+        <v>9.01</v>
+      </c>
+      <c r="C193" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="D193" s="1">
+        <v>2.27</v>
+      </c>
+      <c r="E193" s="1">
+        <v>0</v>
+      </c>
+      <c r="F193" s="1">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A194" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B194" s="1">
+        <v>6.37</v>
+      </c>
+      <c r="C194" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="D194" s="1">
+        <v>1.58</v>
+      </c>
+      <c r="E194" s="1">
+        <v>0</v>
+      </c>
+      <c r="F194" s="1">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A195" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B195" s="1">
+        <v>18.510000000000002</v>
+      </c>
+      <c r="C195" s="1">
+        <v>1</v>
+      </c>
+      <c r="D195" s="1">
+        <v>1.57</v>
+      </c>
+      <c r="E195" s="1">
+        <v>0</v>
+      </c>
+      <c r="F195" s="1">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B196" s="1">
+        <v>9.75</v>
+      </c>
+      <c r="C196" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="D196" s="1">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="E196" s="1">
+        <v>0</v>
+      </c>
+      <c r="F196" s="1">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A197" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B197" s="1">
+        <v>10.91</v>
+      </c>
+      <c r="C197" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="D197" s="1">
+        <v>1.87</v>
+      </c>
+      <c r="E197" s="1">
+        <v>0</v>
+      </c>
+      <c r="F197" s="1">
+        <f>ROUND((F193+F194+F195+F196)/4,2)</f>
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A200" s="1">
+        <v>78.260000000000005</v>
+      </c>
+      <c r="B200" s="1">
+        <v>95.71</v>
+      </c>
+      <c r="C200" s="1">
+        <v>75.94</v>
+      </c>
+      <c r="D200" s="1">
+        <v>76.48</v>
+      </c>
+      <c r="E200" s="1">
+        <v>76.400000000000006</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A201" s="1">
+        <v>10.91</v>
+      </c>
+      <c r="B201" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="C201" s="1">
+        <v>1.87</v>
+      </c>
+      <c r="D201" s="1">
+        <v>0</v>
+      </c>
+      <c r="E201" s="1">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A191:B191"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>